<commit_message>
Updated podcast and mongo data
</commit_message>
<xml_diff>
--- a/assets/testdata/2018-games.xlsx
+++ b/assets/testdata/2018-games.xlsx
@@ -5,26 +5,26 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aronc004/Desktop/github/crowdsourcedscores-web/assets/testdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chrisaronchick/GitHub/crowdsourcedscores-web/assets/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CD193FC-4850-7145-9795-04BB6505E47F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26DD46AC-4DA7-894A-A446-7B832385F98B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
     <sheet name="2018-games" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="18" r:id="rId3"/>
+    <pivotCache cacheId="33" r:id="rId3"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="97">
   <si>
     <t>gameId</t>
   </si>
@@ -257,9 +257,6 @@
     <t>Sum of crowd.results.spread.correct</t>
   </si>
   <si>
-    <t>Sum of crowd.results.winner.correct</t>
-  </si>
-  <si>
     <t>2018-09-28T00:20:00.000Z</t>
   </si>
   <si>
@@ -291,6 +288,33 @@
   </si>
   <si>
     <t>2018-10-08T00:20:00.000Z</t>
+  </si>
+  <si>
+    <t>2018-10-09T00:15:00.000Z</t>
+  </si>
+  <si>
+    <t>2018-10-12T00:20:00.000Z</t>
+  </si>
+  <si>
+    <t>2018-10-14T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>2018-10-14T20:05:00.000Z</t>
+  </si>
+  <si>
+    <t>2018-10-14T20:25:00.000Z</t>
+  </si>
+  <si>
+    <t>2018-10-15T00:20:00.000Z</t>
+  </si>
+  <si>
+    <t>2018-10-16T00:15:00.000Z</t>
+  </si>
+  <si>
+    <t>Sum of crowd.results.spread.push</t>
+  </si>
+  <si>
+    <t>Sum of crowd.results.total.push</t>
   </si>
 </sst>
 </file>
@@ -840,13 +864,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Aronchick, Chris X.-ND" refreshedDate="43367.590686226853" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="48" xr:uid="{00000000-000A-0000-FFFF-FFFF0A000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Gemma and Chris Aronchick" refreshedDate="43388.890694907408" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="93" xr:uid="{00000000-000A-0000-FFFF-FFFF0A000000}">
   <cacheSource type="worksheet">
     <worksheetSource name="Games"/>
   </cacheSource>
   <cacheFields count="21">
     <cacheField name="gameId" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="48" count="48">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="93" count="93">
         <n v="1"/>
         <n v="2"/>
         <n v="3"/>
@@ -895,20 +919,101 @@
         <n v="46"/>
         <n v="47"/>
         <n v="48"/>
+        <n v="49"/>
+        <n v="50"/>
+        <n v="51"/>
+        <n v="52"/>
+        <n v="53"/>
+        <n v="54"/>
+        <n v="55"/>
+        <n v="56"/>
+        <n v="57"/>
+        <n v="58"/>
+        <n v="59"/>
+        <n v="60"/>
+        <n v="61"/>
+        <n v="62"/>
+        <n v="63"/>
+        <n v="64"/>
+        <n v="65"/>
+        <n v="66"/>
+        <n v="67"/>
+        <n v="68"/>
+        <n v="69"/>
+        <n v="70"/>
+        <n v="71"/>
+        <n v="72"/>
+        <n v="73"/>
+        <n v="74"/>
+        <n v="75"/>
+        <n v="76"/>
+        <n v="77"/>
+        <n v="78"/>
+        <n v="79"/>
+        <n v="80"/>
+        <n v="81"/>
+        <n v="82"/>
+        <n v="83"/>
+        <n v="84"/>
+        <n v="85"/>
+        <n v="86"/>
+        <n v="87"/>
+        <n v="88"/>
+        <n v="89"/>
+        <n v="90"/>
+        <n v="91"/>
+        <n v="92"/>
+        <n v="93"/>
       </sharedItems>
     </cacheField>
     <cacheField name="year" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2018" maxValue="2018"/>
     </cacheField>
     <cacheField name="gameWeek" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="3" count="3">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="6" count="6">
         <n v="1"/>
         <n v="2"/>
         <n v="3"/>
+        <n v="4"/>
+        <n v="5"/>
+        <n v="6"/>
       </sharedItems>
     </cacheField>
     <cacheField name="awayTeam.fullName" numFmtId="0">
-      <sharedItems/>
+      <sharedItems count="32">
+        <s v="Atlanta Falcons"/>
+        <s v="Pittsburgh Steelers"/>
+        <s v="Cincinnati Bengals"/>
+        <s v="Tennessee Titans"/>
+        <s v="San Francisco 49ers"/>
+        <s v="Buffalo Bills"/>
+        <s v="Houston Texans"/>
+        <s v="Jacksonville Jaguars"/>
+        <s v="Tampa Bay Buccaneers"/>
+        <s v="Kansas City Chiefs"/>
+        <s v="Washington Redskins"/>
+        <s v="Seattle Seahawks"/>
+        <s v="Dallas Cowboys"/>
+        <s v="Chicago Bears"/>
+        <s v="New York Jets"/>
+        <s v="Los Angeles Rams"/>
+        <s v="Baltimore Ravens"/>
+        <s v="Minnesota Vikings"/>
+        <s v="Cleveland Browns"/>
+        <s v="Miami Dolphins"/>
+        <s v="Los Angeles Chargers"/>
+        <s v="Carolina Panthers"/>
+        <s v="Indianapolis Colts"/>
+        <s v="Philadelphia Eagles"/>
+        <s v="Detroit Lions"/>
+        <s v="Arizona Cardinals"/>
+        <s v="Oakland Raiders"/>
+        <s v="New England Patriots"/>
+        <s v="New York Giants"/>
+        <s v="Denver Broncos"/>
+        <s v="New Orleans Saints"/>
+        <s v="Green Bay Packers"/>
+      </sharedItems>
     </cacheField>
     <cacheField name="homeTeam.fullName" numFmtId="0">
       <sharedItems/>
@@ -917,46 +1022,52 @@
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-16.5" maxValue="7.5"/>
     </cacheField>
     <cacheField name="odds.total" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="39" maxValue="55"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="38.5" maxValue="58.5"/>
     </cacheField>
     <cacheField name="crowd.awayTeam.score" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="9.42" maxValue="30.43"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="9.42" maxValue="30.91"/>
     </cacheField>
     <cacheField name="crowd.homeTeam.score" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="14.36" maxValue="29.15"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="13.6" maxValue="31.18"/>
     </cacheField>
     <cacheField name="crowd.results.winner.correct" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="0" maxValue="1"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="1" count="2">
+        <n v="1"/>
+        <n v="0"/>
+      </sharedItems>
     </cacheField>
     <cacheField name="crowd.results.winner.push" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="0" maxValue="1"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="1"/>
     </cacheField>
     <cacheField name="crowd.results.spread.correct" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="0" maxValue="1"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="1"/>
     </cacheField>
     <cacheField name="crowd.results.spread.push" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="0" maxValue="1"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="1" count="2">
+        <n v="0"/>
+        <n v="1"/>
+      </sharedItems>
     </cacheField>
     <cacheField name="crowd.results.total.correct" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="0" maxValue="1"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="1"/>
     </cacheField>
     <cacheField name="crowd.results.total.push" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="0" maxValue="0"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="1"/>
     </cacheField>
     <cacheField name="crowd.results.predictionScore" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="0" maxValue="6"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="6"/>
     </cacheField>
     <cacheField name="results.awayTeam.score" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="0" maxValue="48"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="48"/>
     </cacheField>
     <cacheField name="results.homeTeam.score" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="6" maxValue="47"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="48"/>
     </cacheField>
     <cacheField name="results.total" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="15" maxValue="88"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="15" maxValue="88"/>
     </cacheField>
     <cacheField name="results.spread" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="-44" maxValue="31"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="-44" maxValue="31"/>
     </cacheField>
     <cacheField name="startDateTime" numFmtId="0">
       <sharedItems/>
@@ -971,21 +1082,21 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="48">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="93">
   <r>
     <x v="0"/>
     <n v="2018"/>
     <x v="0"/>
-    <s v="Atlanta Falcons"/>
+    <x v="0"/>
     <s v="Philadelphia Eagles"/>
     <n v="-1.5"/>
     <n v="44.5"/>
     <n v="20.64"/>
     <n v="23.21"/>
+    <x v="0"/>
+    <n v="0"/>
     <n v="1"/>
-    <n v="0"/>
-    <n v="1"/>
-    <n v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <n v="0"/>
     <n v="6"/>
@@ -999,16 +1110,16 @@
     <x v="1"/>
     <n v="2018"/>
     <x v="0"/>
-    <s v="Pittsburgh Steelers"/>
+    <x v="1"/>
     <s v="Cleveland Browns"/>
     <n v="3.5"/>
     <n v="41"/>
     <n v="26.67"/>
     <n v="17.829999999999998"/>
-    <n v="0"/>
+    <x v="1"/>
     <n v="1"/>
     <n v="0"/>
-    <n v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <n v="0"/>
     <n v="2"/>
@@ -1022,16 +1133,16 @@
     <x v="2"/>
     <n v="2018"/>
     <x v="0"/>
-    <s v="Cincinnati Bengals"/>
+    <x v="2"/>
     <s v="Indianapolis Colts"/>
     <n v="-1"/>
     <n v="47.5"/>
     <n v="17.329999999999998"/>
     <n v="19.670000000000002"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
+    <x v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="0"/>
     <n v="0"/>
     <n v="0"/>
     <n v="0"/>
@@ -1045,16 +1156,16 @@
     <x v="3"/>
     <n v="2018"/>
     <x v="0"/>
-    <s v="Tennessee Titans"/>
+    <x v="3"/>
     <s v="Miami Dolphins"/>
     <n v="-1"/>
     <n v="43.5"/>
     <n v="18.75"/>
     <n v="18.25"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
+    <x v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="0"/>
     <n v="0"/>
     <n v="0"/>
     <n v="0"/>
@@ -1068,16 +1179,16 @@
     <x v="4"/>
     <n v="2018"/>
     <x v="0"/>
-    <s v="San Francisco 49ers"/>
+    <x v="4"/>
     <s v="Minnesota Vikings"/>
     <n v="-6"/>
     <n v="46.5"/>
     <n v="17.170000000000002"/>
     <n v="22.33"/>
-    <n v="1"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <n v="0"/>
     <n v="4"/>
@@ -1091,16 +1202,16 @@
     <x v="5"/>
     <n v="2018"/>
     <x v="0"/>
-    <s v="Buffalo Bills"/>
+    <x v="5"/>
     <s v="Baltimore Ravens"/>
     <n v="-7.5"/>
     <n v="39"/>
     <n v="13.92"/>
     <n v="17.920000000000002"/>
-    <n v="1"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="0"/>
     <n v="0"/>
     <n v="0"/>
     <n v="2"/>
@@ -1114,16 +1225,16 @@
     <x v="6"/>
     <n v="2018"/>
     <x v="0"/>
-    <s v="Houston Texans"/>
+    <x v="6"/>
     <s v="New England Patriots"/>
     <n v="-6.5"/>
     <n v="49.5"/>
     <n v="19.57"/>
     <n v="26.64"/>
+    <x v="0"/>
+    <n v="0"/>
     <n v="1"/>
-    <n v="0"/>
-    <n v="1"/>
-    <n v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <n v="0"/>
     <n v="6"/>
@@ -1137,16 +1248,16 @@
     <x v="7"/>
     <n v="2018"/>
     <x v="0"/>
-    <s v="Jacksonville Jaguars"/>
+    <x v="7"/>
     <s v="New York Giants"/>
     <n v="3"/>
     <n v="42.5"/>
     <n v="20.73"/>
     <n v="14.73"/>
+    <x v="0"/>
+    <n v="0"/>
     <n v="1"/>
-    <n v="0"/>
-    <n v="1"/>
-    <n v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <n v="0"/>
     <n v="6"/>
@@ -1160,16 +1271,16 @@
     <x v="8"/>
     <n v="2018"/>
     <x v="0"/>
-    <s v="Tampa Bay Buccaneers"/>
+    <x v="8"/>
     <s v="New Orleans Saints"/>
     <n v="-10"/>
     <n v="49.5"/>
     <n v="14.38"/>
     <n v="25.85"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
+    <x v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="0"/>
     <n v="0"/>
     <n v="0"/>
     <n v="0"/>
@@ -1183,16 +1294,16 @@
     <x v="9"/>
     <n v="2018"/>
     <x v="0"/>
-    <s v="Kansas City Chiefs"/>
+    <x v="9"/>
     <s v="Los Angeles Chargers"/>
     <n v="-3"/>
     <n v="48"/>
     <n v="18.77"/>
     <n v="21.46"/>
-    <n v="0"/>
+    <x v="1"/>
     <n v="0"/>
     <n v="1"/>
-    <n v="0"/>
+    <x v="0"/>
     <n v="0"/>
     <n v="0"/>
     <n v="2"/>
@@ -1206,16 +1317,16 @@
     <x v="10"/>
     <n v="2018"/>
     <x v="0"/>
-    <s v="Washington Redskins"/>
+    <x v="10"/>
     <s v="Arizona Cardinals"/>
     <n v="-2"/>
     <n v="43.5"/>
     <n v="21.15"/>
     <n v="19.38"/>
+    <x v="0"/>
+    <n v="0"/>
     <n v="1"/>
-    <n v="0"/>
-    <n v="1"/>
-    <n v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <n v="0"/>
     <n v="6"/>
@@ -1229,16 +1340,16 @@
     <x v="11"/>
     <n v="2018"/>
     <x v="0"/>
-    <s v="Seattle Seahawks"/>
+    <x v="11"/>
     <s v="Denver Broncos"/>
     <n v="-3"/>
     <n v="42.5"/>
     <n v="20.46"/>
     <n v="19.079999999999998"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="1"/>
+    <x v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="1"/>
     <n v="0"/>
     <n v="0"/>
     <n v="0"/>
@@ -1252,16 +1363,16 @@
     <x v="12"/>
     <n v="2018"/>
     <x v="0"/>
-    <s v="Dallas Cowboys"/>
+    <x v="12"/>
     <s v="Carolina Panthers"/>
     <n v="-3"/>
     <n v="42"/>
     <n v="16.77"/>
     <n v="22.23"/>
+    <x v="0"/>
+    <n v="0"/>
     <n v="1"/>
-    <n v="0"/>
-    <n v="1"/>
-    <n v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <n v="0"/>
     <n v="6"/>
@@ -1275,16 +1386,16 @@
     <x v="13"/>
     <n v="2018"/>
     <x v="0"/>
-    <s v="Chicago Bears"/>
+    <x v="13"/>
     <s v="Green Bay Packers"/>
     <n v="-7"/>
     <n v="46.5"/>
     <n v="16.23"/>
     <n v="25.23"/>
-    <n v="1"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="0"/>
     <n v="0"/>
     <n v="0"/>
     <n v="2"/>
@@ -1298,16 +1409,16 @@
     <x v="14"/>
     <n v="2018"/>
     <x v="0"/>
-    <s v="New York Jets"/>
+    <x v="14"/>
     <s v="Detroit Lions"/>
     <n v="-7"/>
     <n v="44.5"/>
     <n v="17.850000000000001"/>
     <n v="20.62"/>
-    <n v="0"/>
+    <x v="1"/>
     <n v="0"/>
     <n v="1"/>
-    <n v="0"/>
+    <x v="0"/>
     <n v="0"/>
     <n v="0"/>
     <n v="2"/>
@@ -1321,16 +1432,16 @@
     <x v="15"/>
     <n v="2018"/>
     <x v="0"/>
-    <s v="Los Angeles Rams"/>
+    <x v="15"/>
     <s v="Oakland Raiders"/>
     <n v="4.5"/>
     <n v="47.5"/>
     <n v="26.23"/>
     <n v="18.38"/>
+    <x v="0"/>
+    <n v="0"/>
     <n v="1"/>
-    <n v="0"/>
-    <n v="1"/>
-    <n v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <n v="0"/>
     <n v="6"/>
@@ -1344,16 +1455,16 @@
     <x v="16"/>
     <n v="2018"/>
     <x v="1"/>
-    <s v="Baltimore Ravens"/>
+    <x v="16"/>
     <s v="Cincinnati Bengals"/>
     <n v="-1"/>
     <n v="44.5"/>
     <n v="22.33"/>
     <n v="16.75"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
+    <x v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="0"/>
     <n v="0"/>
     <n v="0"/>
     <n v="0"/>
@@ -1367,16 +1478,16 @@
     <x v="17"/>
     <n v="2018"/>
     <x v="1"/>
-    <s v="Minnesota Vikings"/>
+    <x v="17"/>
     <s v="Green Bay Packers"/>
     <n v="2"/>
     <n v="45"/>
     <n v="22.62"/>
     <n v="21.69"/>
-    <n v="0"/>
+    <x v="1"/>
     <n v="1"/>
     <n v="1"/>
-    <n v="0"/>
+    <x v="0"/>
     <n v="0"/>
     <n v="0"/>
     <n v="2"/>
@@ -1390,16 +1501,16 @@
     <x v="18"/>
     <n v="2018"/>
     <x v="1"/>
-    <s v="Cleveland Browns"/>
+    <x v="18"/>
     <s v="New Orleans Saints"/>
     <n v="-9.5"/>
     <n v="51"/>
     <n v="17.149999999999999"/>
     <n v="28.92"/>
-    <n v="1"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <n v="0"/>
     <n v="4"/>
@@ -1413,16 +1524,16 @@
     <x v="19"/>
     <n v="2018"/>
     <x v="1"/>
-    <s v="Miami Dolphins"/>
+    <x v="19"/>
     <s v="New York Jets"/>
     <n v="-3"/>
     <n v="42.5"/>
     <n v="18.420000000000002"/>
     <n v="19.670000000000002"/>
-    <n v="0"/>
+    <x v="1"/>
     <n v="0"/>
     <n v="1"/>
-    <n v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <n v="0"/>
     <n v="4"/>
@@ -1436,16 +1547,16 @@
     <x v="20"/>
     <n v="2018"/>
     <x v="1"/>
-    <s v="Los Angeles Chargers"/>
+    <x v="20"/>
     <s v="Buffalo Bills"/>
     <n v="7.5"/>
     <n v="41.5"/>
     <n v="30.42"/>
     <n v="15.92"/>
+    <x v="0"/>
+    <n v="0"/>
     <n v="1"/>
-    <n v="0"/>
-    <n v="1"/>
-    <n v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <n v="0"/>
     <n v="6"/>
@@ -1459,16 +1570,16 @@
     <x v="21"/>
     <n v="2018"/>
     <x v="1"/>
-    <s v="Carolina Panthers"/>
+    <x v="21"/>
     <s v="Atlanta Falcons"/>
     <n v="-5"/>
     <n v="43.5"/>
     <n v="21.08"/>
     <n v="21.5"/>
-    <n v="1"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="0"/>
     <n v="0"/>
     <n v="0"/>
     <n v="2"/>
@@ -1482,16 +1593,16 @@
     <x v="22"/>
     <n v="2018"/>
     <x v="1"/>
-    <s v="Kansas City Chiefs"/>
+    <x v="9"/>
     <s v="Pittsburgh Steelers"/>
     <n v="-4"/>
     <n v="52.5"/>
     <n v="24.77"/>
     <n v="23.31"/>
+    <x v="0"/>
+    <n v="0"/>
     <n v="1"/>
-    <n v="0"/>
-    <n v="1"/>
-    <n v="0"/>
+    <x v="0"/>
     <n v="0"/>
     <n v="0"/>
     <n v="4"/>
@@ -1505,16 +1616,16 @@
     <x v="23"/>
     <n v="2018"/>
     <x v="1"/>
-    <s v="Indianapolis Colts"/>
+    <x v="22"/>
     <s v="Washington Redskins"/>
     <n v="-6"/>
     <n v="47.5"/>
     <n v="18.309999999999999"/>
     <n v="21.15"/>
-    <n v="0"/>
+    <x v="1"/>
     <n v="0"/>
     <n v="1"/>
-    <n v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <n v="0"/>
     <n v="4"/>
@@ -1528,16 +1639,16 @@
     <x v="24"/>
     <n v="2018"/>
     <x v="1"/>
-    <s v="Houston Texans"/>
+    <x v="6"/>
     <s v="Tennessee Titans"/>
     <n v="3"/>
     <n v="41"/>
     <n v="22.67"/>
     <n v="16.170000000000002"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
+    <x v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <n v="0"/>
     <n v="2"/>
@@ -1551,16 +1662,16 @@
     <x v="25"/>
     <n v="2018"/>
     <x v="1"/>
-    <s v="Philadelphia Eagles"/>
+    <x v="23"/>
     <s v="Tampa Bay Buccaneers"/>
     <n v="3"/>
     <n v="46.5"/>
     <n v="24.23"/>
     <n v="18.079999999999998"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
+    <x v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="0"/>
     <n v="0"/>
     <n v="0"/>
     <n v="0"/>
@@ -1574,16 +1685,16 @@
     <x v="26"/>
     <n v="2018"/>
     <x v="1"/>
-    <s v="Detroit Lions"/>
+    <x v="24"/>
     <s v="San Francisco 49ers"/>
     <n v="-6"/>
     <n v="48"/>
     <n v="19"/>
     <n v="22.58"/>
+    <x v="0"/>
+    <n v="0"/>
     <n v="1"/>
-    <n v="0"/>
-    <n v="1"/>
-    <n v="0"/>
+    <x v="0"/>
     <n v="0"/>
     <n v="0"/>
     <n v="4"/>
@@ -1597,16 +1708,16 @@
     <x v="27"/>
     <n v="2018"/>
     <x v="1"/>
-    <s v="Arizona Cardinals"/>
+    <x v="25"/>
     <s v="Los Angeles Rams"/>
     <n v="-12.5"/>
     <n v="43.5"/>
     <n v="13.42"/>
     <n v="27.25"/>
+    <x v="0"/>
+    <n v="0"/>
     <n v="1"/>
-    <n v="0"/>
-    <n v="1"/>
-    <n v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <n v="0"/>
     <n v="6"/>
@@ -1620,16 +1731,16 @@
     <x v="28"/>
     <n v="2018"/>
     <x v="1"/>
-    <s v="Oakland Raiders"/>
+    <x v="26"/>
     <s v="Denver Broncos"/>
     <n v="-6.5"/>
     <n v="44.5"/>
     <n v="17.329999999999998"/>
     <n v="22"/>
+    <x v="0"/>
+    <n v="0"/>
     <n v="1"/>
-    <n v="0"/>
-    <n v="1"/>
-    <n v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <n v="0"/>
     <n v="6"/>
@@ -1643,16 +1754,16 @@
     <x v="29"/>
     <n v="2018"/>
     <x v="1"/>
-    <s v="New England Patriots"/>
+    <x v="27"/>
     <s v="Jacksonville Jaguars"/>
     <n v="1.5"/>
     <n v="44"/>
     <n v="24.33"/>
     <n v="20.25"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
+    <x v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <n v="0"/>
     <n v="2"/>
@@ -1666,16 +1777,16 @@
     <x v="30"/>
     <n v="2018"/>
     <x v="1"/>
-    <s v="New York Giants"/>
+    <x v="28"/>
     <s v="Dallas Cowboys"/>
     <n v="-3"/>
     <n v="42"/>
     <n v="19.25"/>
     <n v="20.5"/>
-    <n v="1"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <n v="0"/>
     <n v="4"/>
@@ -1689,16 +1800,16 @@
     <x v="31"/>
     <n v="2018"/>
     <x v="1"/>
-    <s v="Seattle Seahawks"/>
+    <x v="11"/>
     <s v="Chicago Bears"/>
     <n v="-3.5"/>
     <n v="43"/>
     <n v="22.45"/>
     <n v="22.55"/>
-    <n v="1"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="0"/>
     <n v="0"/>
     <n v="0"/>
     <n v="2"/>
@@ -1712,16 +1823,16 @@
     <x v="32"/>
     <n v="2018"/>
     <x v="2"/>
-    <s v="New York Jets"/>
+    <x v="14"/>
     <s v="Cleveland Browns"/>
     <n v="-3"/>
     <n v="41"/>
     <n v="18.89"/>
     <n v="19.559999999999999"/>
-    <n v="1"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <n v="0"/>
     <n v="4"/>
@@ -1735,16 +1846,16 @@
     <x v="33"/>
     <n v="2018"/>
     <x v="2"/>
-    <s v="Cincinnati Bengals"/>
+    <x v="2"/>
     <s v="Carolina Panthers"/>
     <n v="-2.5"/>
     <n v="44"/>
     <n v="20.079999999999998"/>
     <n v="23.38"/>
+    <x v="0"/>
+    <n v="0"/>
     <n v="1"/>
-    <n v="0"/>
-    <n v="1"/>
-    <n v="0"/>
+    <x v="0"/>
     <n v="0"/>
     <n v="0"/>
     <n v="4"/>
@@ -1758,16 +1869,16 @@
     <x v="34"/>
     <n v="2018"/>
     <x v="2"/>
-    <s v="New York Giants"/>
+    <x v="28"/>
     <s v="Houston Texans"/>
     <n v="-6"/>
     <n v="44"/>
     <n v="14.31"/>
     <n v="20.46"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
+    <x v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="0"/>
     <n v="0"/>
     <n v="0"/>
     <n v="0"/>
@@ -1781,16 +1892,16 @@
     <x v="35"/>
     <n v="2018"/>
     <x v="2"/>
-    <s v="Tennessee Titans"/>
+    <x v="3"/>
     <s v="Jacksonville Jaguars"/>
     <n v="-10"/>
     <n v="39.5"/>
     <n v="13.77"/>
     <n v="24.08"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
+    <x v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <n v="0"/>
     <n v="2"/>
@@ -1804,16 +1915,16 @@
     <x v="36"/>
     <n v="2018"/>
     <x v="2"/>
-    <s v="Denver Broncos"/>
+    <x v="29"/>
     <s v="Baltimore Ravens"/>
     <n v="-5.5"/>
     <n v="46"/>
     <n v="18.62"/>
     <n v="20.38"/>
-    <n v="1"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <n v="0"/>
     <n v="4"/>
@@ -1827,16 +1938,16 @@
     <x v="37"/>
     <n v="2018"/>
     <x v="2"/>
-    <s v="New Orleans Saints"/>
+    <x v="30"/>
     <s v="Atlanta Falcons"/>
     <n v="-1.5"/>
     <n v="53.5"/>
     <n v="26.5"/>
     <n v="26.5"/>
-    <n v="0"/>
+    <x v="1"/>
     <n v="0"/>
     <n v="1"/>
-    <n v="0"/>
+    <x v="0"/>
     <n v="0"/>
     <n v="0"/>
     <n v="2"/>
@@ -1850,16 +1961,16 @@
     <x v="38"/>
     <n v="2018"/>
     <x v="2"/>
-    <s v="San Francisco 49ers"/>
+    <x v="4"/>
     <s v="Kansas City Chiefs"/>
     <n v="-5.5"/>
     <n v="53.5"/>
     <n v="21.08"/>
     <n v="29.15"/>
+    <x v="0"/>
+    <n v="0"/>
     <n v="1"/>
-    <n v="0"/>
-    <n v="1"/>
-    <n v="0"/>
+    <x v="0"/>
     <n v="0"/>
     <n v="0"/>
     <n v="4"/>
@@ -1873,16 +1984,16 @@
     <x v="39"/>
     <n v="2018"/>
     <x v="2"/>
-    <s v="Green Bay Packers"/>
+    <x v="31"/>
     <s v="Washington Redskins"/>
     <n v="2.5"/>
     <n v="45.5"/>
     <n v="25.77"/>
     <n v="19.62"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
+    <x v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="0"/>
     <n v="0"/>
     <n v="0"/>
     <n v="0"/>
@@ -1896,16 +2007,16 @@
     <x v="40"/>
     <n v="2018"/>
     <x v="2"/>
-    <s v="Indianapolis Colts"/>
+    <x v="22"/>
     <s v="Philadelphia Eagles"/>
     <n v="-6.5"/>
     <n v="45.5"/>
     <n v="19.77"/>
     <n v="26.62"/>
-    <n v="1"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="0"/>
     <n v="0"/>
     <n v="0"/>
     <n v="2"/>
@@ -1919,16 +2030,16 @@
     <x v="41"/>
     <n v="2018"/>
     <x v="2"/>
-    <s v="Oakland Raiders"/>
+    <x v="26"/>
     <s v="Miami Dolphins"/>
     <n v="-3"/>
     <n v="44.5"/>
     <n v="17.079999999999998"/>
     <n v="20.77"/>
+    <x v="0"/>
+    <n v="0"/>
     <n v="1"/>
-    <n v="0"/>
-    <n v="1"/>
-    <n v="0"/>
+    <x v="0"/>
     <n v="0"/>
     <n v="0"/>
     <n v="4"/>
@@ -1942,16 +2053,16 @@
     <x v="42"/>
     <n v="2018"/>
     <x v="2"/>
-    <s v="Buffalo Bills"/>
+    <x v="5"/>
     <s v="Minnesota Vikings"/>
     <n v="-16.5"/>
     <n v="41"/>
     <n v="9.42"/>
     <n v="26"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
+    <x v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <n v="0"/>
     <n v="2"/>
@@ -1965,16 +2076,16 @@
     <x v="43"/>
     <n v="2018"/>
     <x v="2"/>
-    <s v="Los Angeles Chargers"/>
+    <x v="20"/>
     <s v="Los Angeles Rams"/>
     <n v="-7"/>
     <n v="49"/>
     <n v="23.08"/>
     <n v="28.83"/>
-    <n v="1"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <n v="0"/>
     <n v="4"/>
@@ -1988,16 +2099,16 @@
     <x v="44"/>
     <n v="2018"/>
     <x v="2"/>
-    <s v="Chicago Bears"/>
+    <x v="13"/>
     <s v="Arizona Cardinals"/>
     <n v="6"/>
     <n v="39"/>
     <n v="22.43"/>
     <n v="14.36"/>
-    <n v="1"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <n v="0"/>
     <n v="4"/>
@@ -2011,16 +2122,16 @@
     <x v="45"/>
     <n v="2018"/>
     <x v="2"/>
-    <s v="Dallas Cowboys"/>
+    <x v="12"/>
     <s v="Seattle Seahawks"/>
     <n v="-1"/>
     <n v="40"/>
     <n v="20.93"/>
     <n v="22"/>
+    <x v="0"/>
+    <n v="0"/>
     <n v="1"/>
-    <n v="0"/>
-    <n v="1"/>
-    <n v="0"/>
+    <x v="0"/>
     <n v="0"/>
     <n v="0"/>
     <n v="4"/>
@@ -2034,16 +2145,16 @@
     <x v="46"/>
     <n v="2018"/>
     <x v="2"/>
-    <s v="New England Patriots"/>
+    <x v="27"/>
     <s v="Detroit Lions"/>
     <n v="6.5"/>
     <n v="55"/>
     <n v="30.43"/>
     <n v="15.93"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
+    <x v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <n v="0"/>
     <n v="2"/>
@@ -2057,34 +2168,1069 @@
     <x v="47"/>
     <n v="2018"/>
     <x v="2"/>
-    <s v="Pittsburgh Steelers"/>
+    <x v="1"/>
     <s v="Tampa Bay Buccaneers"/>
     <n v="-1.5"/>
     <n v="54.5"/>
     <n v="28.07"/>
     <n v="26.43"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="1"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="4"/>
+    <n v="30"/>
+    <n v="27"/>
+    <n v="57"/>
+    <n v="3"/>
     <s v="2018-09-25T00:15:00.000Z"/>
+  </r>
+  <r>
+    <x v="48"/>
+    <n v="2018"/>
+    <x v="3"/>
+    <x v="17"/>
+    <s v="Los Angeles Rams"/>
+    <n v="-7"/>
+    <n v="48.5"/>
+    <n v="21.07"/>
+    <n v="29.4"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="4"/>
+    <n v="31"/>
+    <n v="38"/>
+    <n v="69"/>
+    <n v="-7"/>
+    <s v="2018-09-28T00:20:00.000Z"/>
+  </r>
+  <r>
+    <x v="49"/>
+    <n v="2018"/>
+    <x v="3"/>
+    <x v="24"/>
+    <s v="Dallas Cowboys"/>
+    <n v="-2.5"/>
+    <n v="44"/>
+    <n v="21.71"/>
+    <n v="19.29"/>
+    <x v="1"/>
+    <n v="0"/>
+    <n v="1"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
+    <n v="24"/>
+    <n v="26"/>
+    <n v="50"/>
+    <n v="-2"/>
+    <s v="2018-09-30T17:00:00.000Z"/>
+  </r>
+  <r>
+    <x v="50"/>
+    <n v="2018"/>
+    <x v="3"/>
+    <x v="5"/>
+    <s v="Green Bay Packers"/>
+    <n v="-9"/>
+    <n v="43.5"/>
+    <n v="16.5"/>
+    <n v="27.57"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="1"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="4"/>
+    <n v="0"/>
+    <n v="22"/>
+    <n v="22"/>
+    <n v="-22"/>
+    <s v="2018-09-30T17:00:00.000Z"/>
+  </r>
+  <r>
+    <x v="51"/>
+    <n v="2018"/>
+    <x v="3"/>
+    <x v="6"/>
+    <s v="Indianapolis Colts"/>
+    <n v="1"/>
+    <n v="48"/>
+    <n v="20.29"/>
+    <n v="22.93"/>
+    <x v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="37"/>
+    <n v="34"/>
+    <n v="71"/>
+    <n v="3"/>
+    <s v="2018-09-30T17:00:00.000Z"/>
+  </r>
+  <r>
+    <x v="52"/>
+    <n v="2018"/>
+    <x v="3"/>
+    <x v="8"/>
+    <s v="Chicago Bears"/>
+    <n v="-3"/>
+    <n v="46"/>
+    <n v="21.79"/>
+    <n v="19.79"/>
+    <x v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="10"/>
+    <n v="48"/>
+    <n v="58"/>
+    <n v="-38"/>
+    <s v="2018-09-30T17:00:00.000Z"/>
+  </r>
+  <r>
+    <x v="53"/>
+    <n v="2018"/>
+    <x v="3"/>
+    <x v="2"/>
+    <s v="Atlanta Falcons"/>
+    <n v="-3.5"/>
+    <n v="52.5"/>
+    <n v="22.64"/>
+    <n v="27.57"/>
+    <x v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="37"/>
+    <n v="36"/>
+    <n v="73"/>
+    <n v="1"/>
+    <s v="2018-09-30T17:00:00.000Z"/>
+  </r>
+  <r>
+    <x v="54"/>
+    <n v="2018"/>
+    <x v="3"/>
+    <x v="14"/>
+    <s v="Jacksonville Jaguars"/>
+    <n v="-7"/>
+    <n v="40"/>
+    <n v="14.64"/>
+    <n v="23.07"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="1"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="4"/>
+    <n v="12"/>
+    <n v="31"/>
+    <n v="43"/>
+    <n v="-19"/>
+    <s v="2018-09-30T17:00:00.000Z"/>
+  </r>
+  <r>
+    <x v="55"/>
+    <n v="2018"/>
+    <x v="3"/>
+    <x v="23"/>
+    <s v="Tennessee Titans"/>
+    <n v="3"/>
+    <n v="41"/>
+    <n v="24.13"/>
+    <n v="17.07"/>
+    <x v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="2"/>
+    <n v="23"/>
+    <n v="26"/>
+    <n v="49"/>
+    <n v="-3"/>
+    <s v="2018-09-30T17:00:00.000Z"/>
+  </r>
+  <r>
+    <x v="56"/>
+    <n v="2018"/>
+    <x v="3"/>
+    <x v="19"/>
+    <s v="New England Patriots"/>
+    <n v="-6.5"/>
+    <n v="50.5"/>
+    <n v="18.329999999999998"/>
+    <n v="23.53"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="4"/>
+    <n v="7"/>
+    <n v="38"/>
+    <n v="45"/>
+    <n v="-31"/>
+    <s v="2018-09-30T17:00:00.000Z"/>
+  </r>
+  <r>
+    <x v="57"/>
+    <n v="2018"/>
+    <x v="3"/>
+    <x v="11"/>
+    <s v="Arizona Cardinals"/>
+    <n v="3.5"/>
+    <n v="40"/>
+    <n v="24.47"/>
+    <n v="15.2"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="4"/>
+    <n v="20"/>
+    <n v="17"/>
+    <n v="37"/>
+    <n v="3"/>
+    <s v="2018-09-30T20:05:00.000Z"/>
+  </r>
+  <r>
+    <x v="58"/>
+    <n v="2018"/>
+    <x v="3"/>
+    <x v="18"/>
+    <s v="Oakland Raiders"/>
+    <n v="-2.5"/>
+    <n v="44.5"/>
+    <n v="20.399999999999999"/>
+    <n v="17.73"/>
+    <x v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="42"/>
+    <n v="45"/>
+    <n v="87"/>
+    <n v="-3"/>
+    <s v="2018-09-30T20:05:00.000Z"/>
+  </r>
+  <r>
+    <x v="59"/>
+    <n v="2018"/>
+    <x v="3"/>
+    <x v="30"/>
+    <s v="New York Giants"/>
+    <n v="3"/>
+    <n v="52"/>
+    <n v="27.93"/>
+    <n v="20.53"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="1"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="6"/>
+    <n v="33"/>
+    <n v="18"/>
+    <n v="51"/>
+    <n v="15"/>
+    <s v="2018-09-30T20:25:00.000Z"/>
+  </r>
+  <r>
+    <x v="60"/>
+    <n v="2018"/>
+    <x v="3"/>
+    <x v="4"/>
+    <s v="Los Angeles Chargers"/>
+    <n v="-10"/>
+    <n v="46"/>
+    <n v="14.07"/>
+    <n v="29.73"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
+    <n v="27"/>
+    <n v="29"/>
+    <n v="56"/>
+    <n v="-2"/>
+    <s v="2018-09-30T20:25:00.000Z"/>
+  </r>
+  <r>
+    <x v="61"/>
+    <n v="2018"/>
+    <x v="3"/>
+    <x v="16"/>
+    <s v="Pittsburgh Steelers"/>
+    <n v="-3"/>
+    <n v="51"/>
+    <n v="21.4"/>
+    <n v="25.33"/>
+    <x v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="2"/>
+    <n v="26"/>
+    <n v="14"/>
+    <n v="40"/>
+    <n v="12"/>
+    <s v="2018-10-01T00:20:00.000Z"/>
+  </r>
+  <r>
+    <x v="62"/>
+    <n v="2018"/>
+    <x v="3"/>
+    <x v="9"/>
+    <s v="Denver Broncos"/>
+    <n v="3.5"/>
+    <n v="53.5"/>
+    <n v="29.47"/>
+    <n v="23.27"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="1"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="6"/>
+    <n v="27"/>
+    <n v="23"/>
+    <n v="50"/>
+    <n v="4"/>
+    <s v="2018-10-02T00:15:00.000Z"/>
+  </r>
+  <r>
+    <x v="63"/>
+    <n v="2018"/>
+    <x v="4"/>
+    <x v="22"/>
+    <s v="New England Patriots"/>
+    <n v="-10.5"/>
+    <n v="50.5"/>
+    <n v="19.920000000000002"/>
+    <n v="30.69"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="1"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="6"/>
+    <n v="24"/>
+    <n v="38"/>
+    <n v="62"/>
+    <n v="-14"/>
+    <s v="2018-10-05T00:20:00.000Z"/>
+  </r>
+  <r>
+    <x v="64"/>
+    <n v="2018"/>
+    <x v="4"/>
+    <x v="19"/>
+    <s v="Cincinnati Bengals"/>
+    <n v="-6"/>
+    <n v="47.5"/>
+    <n v="20.67"/>
+    <n v="25.87"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="4"/>
+    <n v="17"/>
+    <n v="27"/>
+    <n v="44"/>
+    <n v="-10"/>
+    <s v="2018-10-07T17:00:00.000Z"/>
+  </r>
+  <r>
+    <x v="65"/>
+    <n v="2018"/>
+    <x v="4"/>
+    <x v="16"/>
+    <s v="Cleveland Browns"/>
+    <n v="3"/>
+    <n v="45"/>
+    <n v="23.33"/>
+    <n v="20.53"/>
+    <x v="1"/>
+    <n v="0"/>
+    <n v="1"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="4"/>
+    <n v="9"/>
+    <n v="12"/>
+    <n v="21"/>
+    <n v="-3"/>
+    <s v="2018-10-07T17:00:00.000Z"/>
+  </r>
+  <r>
+    <x v="66"/>
+    <n v="2018"/>
+    <x v="4"/>
+    <x v="28"/>
+    <s v="Carolina Panthers"/>
+    <n v="-6.5"/>
+    <n v="43.5"/>
+    <n v="14.43"/>
+    <n v="25.36"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
+    <n v="31"/>
+    <n v="33"/>
+    <n v="64"/>
+    <n v="-2"/>
+    <s v="2018-10-07T17:00:00.000Z"/>
+  </r>
+  <r>
+    <x v="67"/>
+    <n v="2018"/>
+    <x v="4"/>
+    <x v="3"/>
+    <s v="Buffalo Bills"/>
+    <n v="5.5"/>
+    <n v="38.5"/>
+    <n v="23.13"/>
+    <n v="13.6"/>
+    <x v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="2"/>
+    <n v="12"/>
+    <n v="13"/>
+    <n v="25"/>
+    <n v="-1"/>
+    <s v="2018-10-07T17:00:00.000Z"/>
+  </r>
+  <r>
+    <x v="68"/>
+    <n v="2018"/>
+    <x v="4"/>
+    <x v="31"/>
+    <s v="Detroit Lions"/>
+    <n v="1"/>
+    <n v="50"/>
+    <n v="27.13"/>
+    <n v="24"/>
+    <x v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="2"/>
+    <n v="23"/>
+    <n v="31"/>
+    <n v="54"/>
+    <n v="-8"/>
+    <s v="2018-10-07T17:00:00.000Z"/>
+  </r>
+  <r>
+    <x v="69"/>
+    <n v="2018"/>
+    <x v="4"/>
+    <x v="0"/>
+    <s v="Pittsburgh Steelers"/>
+    <n v="-3.5"/>
+    <n v="57"/>
+    <n v="26.2"/>
+    <n v="26.8"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
+    <n v="17"/>
+    <n v="41"/>
+    <n v="58"/>
+    <n v="-24"/>
+    <s v="2018-10-07T17:00:00.000Z"/>
+  </r>
+  <r>
+    <x v="70"/>
+    <n v="2018"/>
+    <x v="4"/>
+    <x v="29"/>
+    <s v="New York Jets"/>
+    <n v="-1"/>
+    <n v="42.5"/>
+    <n v="22.31"/>
+    <n v="16"/>
+    <x v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="16"/>
+    <n v="34"/>
+    <n v="50"/>
+    <n v="-18"/>
+    <s v="2018-10-07T17:00:00.000Z"/>
+  </r>
+  <r>
+    <x v="71"/>
+    <n v="2018"/>
+    <x v="4"/>
+    <x v="7"/>
+    <s v="Kansas City Chiefs"/>
+    <n v="-3"/>
+    <n v="48.5"/>
+    <n v="21.25"/>
+    <n v="25.94"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="1"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="6"/>
+    <n v="14"/>
+    <n v="30"/>
+    <n v="44"/>
+    <n v="-16"/>
+    <s v="2018-10-07T17:00:00.000Z"/>
+  </r>
+  <r>
+    <x v="72"/>
+    <n v="2018"/>
+    <x v="4"/>
+    <x v="26"/>
+    <s v="Los Angeles Chargers"/>
+    <n v="-5"/>
+    <n v="51.5"/>
+    <n v="19.670000000000002"/>
+    <n v="27.27"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="1"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="6"/>
+    <n v="10"/>
+    <n v="26"/>
+    <n v="36"/>
+    <n v="-16"/>
+    <s v="2018-10-07T20:05:00.000Z"/>
+  </r>
+  <r>
+    <x v="73"/>
+    <n v="2018"/>
+    <x v="4"/>
+    <x v="25"/>
+    <s v="San Francisco 49ers"/>
+    <n v="-3"/>
+    <n v="40.5"/>
+    <n v="18.27"/>
+    <n v="19.670000000000002"/>
+    <x v="1"/>
+    <n v="0"/>
+    <n v="1"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
+    <n v="28"/>
+    <n v="18"/>
+    <n v="46"/>
+    <n v="10"/>
+    <s v="2018-10-07T20:25:00.000Z"/>
+  </r>
+  <r>
+    <x v="74"/>
+    <n v="2018"/>
+    <x v="4"/>
+    <x v="17"/>
+    <s v="Philadelphia Eagles"/>
+    <n v="-3"/>
+    <n v="48"/>
+    <n v="22.27"/>
+    <n v="23.47"/>
+    <x v="1"/>
+    <n v="0"/>
+    <n v="1"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="4"/>
+    <n v="23"/>
+    <n v="21"/>
+    <n v="44"/>
+    <n v="2"/>
+    <s v="2018-10-07T20:25:00.000Z"/>
+  </r>
+  <r>
+    <x v="75"/>
+    <n v="2018"/>
+    <x v="4"/>
+    <x v="15"/>
+    <s v="Seattle Seahawks"/>
+    <n v="7.5"/>
+    <n v="50"/>
+    <n v="27.6"/>
+    <n v="21.87"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="1"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="4"/>
+    <n v="33"/>
+    <n v="31"/>
+    <n v="64"/>
+    <n v="2"/>
+    <s v="2018-10-07T20:25:00.000Z"/>
+  </r>
+  <r>
+    <x v="76"/>
+    <n v="2018"/>
+    <x v="4"/>
+    <x v="12"/>
+    <s v="Houston Texans"/>
+    <n v="-3"/>
+    <n v="45.5"/>
+    <n v="20.64"/>
+    <n v="22.86"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="4"/>
+    <n v="16"/>
+    <n v="19"/>
+    <n v="35"/>
+    <n v="-3"/>
+    <s v="2018-10-08T00:20:00.000Z"/>
+  </r>
+  <r>
+    <x v="77"/>
+    <n v="2018"/>
+    <x v="4"/>
+    <x v="10"/>
+    <s v="New Orleans Saints"/>
+    <n v="-6"/>
+    <n v="52.5"/>
+    <n v="22.53"/>
+    <n v="30"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="1"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="6"/>
+    <n v="19"/>
+    <n v="43"/>
+    <n v="62"/>
+    <n v="-24"/>
+    <s v="2018-10-09T00:15:00.000Z"/>
+  </r>
+  <r>
+    <x v="78"/>
+    <n v="2018"/>
+    <x v="5"/>
+    <x v="23"/>
+    <s v="New York Giants"/>
+    <n v="1.5"/>
+    <n v="44"/>
+    <n v="23.75"/>
+    <n v="19.63"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="1"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="4"/>
+    <n v="34"/>
+    <n v="13"/>
+    <n v="47"/>
+    <n v="21"/>
+    <s v="2018-10-12T00:20:00.000Z"/>
+  </r>
+  <r>
+    <x v="79"/>
+    <n v="2018"/>
+    <x v="5"/>
+    <x v="20"/>
+    <s v="Cleveland Browns"/>
+    <n v="-1"/>
+    <n v="47"/>
+    <n v="23"/>
+    <n v="20.73"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="1"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="4"/>
+    <n v="38"/>
+    <n v="14"/>
+    <n v="52"/>
+    <n v="24"/>
+    <s v="2018-10-14T17:00:00.000Z"/>
+  </r>
+  <r>
+    <x v="80"/>
+    <n v="2018"/>
+    <x v="5"/>
+    <x v="5"/>
+    <s v="Houston Texans"/>
+    <n v="-10"/>
+    <n v="40"/>
+    <n v="16.45"/>
+    <n v="23.64"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="1"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="4"/>
+    <n v="13"/>
+    <n v="20"/>
+    <n v="33"/>
+    <n v="-7"/>
+    <s v="2018-10-14T17:00:00.000Z"/>
+  </r>
+  <r>
+    <x v="81"/>
+    <n v="2018"/>
+    <x v="5"/>
+    <x v="1"/>
+    <s v="Cincinnati Bengals"/>
+    <n v="-1.5"/>
+    <n v="50"/>
+    <n v="28.8"/>
+    <n v="28"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="1"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="4"/>
+    <n v="28"/>
+    <n v="21"/>
+    <n v="49"/>
+    <n v="7"/>
+    <s v="2018-10-14T17:00:00.000Z"/>
+  </r>
+  <r>
+    <x v="82"/>
+    <n v="2018"/>
+    <x v="5"/>
+    <x v="8"/>
+    <s v="Atlanta Falcons"/>
+    <n v="-3"/>
+    <n v="57.5"/>
+    <n v="22.73"/>
+    <n v="28.45"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="1"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="4"/>
+    <n v="29"/>
+    <n v="34"/>
+    <n v="63"/>
+    <n v="-5"/>
+    <s v="2018-10-14T17:00:00.000Z"/>
+  </r>
+  <r>
+    <x v="83"/>
+    <n v="2018"/>
+    <x v="5"/>
+    <x v="13"/>
+    <s v="Miami Dolphins"/>
+    <n v="5.5"/>
+    <n v="41.5"/>
+    <n v="22.82"/>
+    <n v="19.36"/>
+    <x v="1"/>
+    <n v="0"/>
+    <n v="1"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="4"/>
+    <n v="28"/>
+    <n v="31"/>
+    <n v="59"/>
+    <n v="-3"/>
+    <s v="2018-10-14T17:00:00.000Z"/>
+  </r>
+  <r>
+    <x v="84"/>
+    <n v="2018"/>
+    <x v="5"/>
+    <x v="21"/>
+    <s v="Washington Redskins"/>
+    <n v="1"/>
+    <n v="44.5"/>
+    <n v="21.64"/>
+    <n v="21"/>
+    <x v="1"/>
+    <n v="0"/>
+    <n v="1"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="4"/>
+    <n v="17"/>
+    <n v="23"/>
+    <n v="40"/>
+    <n v="-6"/>
+    <s v="2018-10-14T17:00:00.000Z"/>
+  </r>
+  <r>
+    <x v="85"/>
+    <n v="2018"/>
+    <x v="5"/>
+    <x v="11"/>
+    <s v="Oakland Raiders"/>
+    <n v="3"/>
+    <n v="48"/>
+    <n v="26.82"/>
+    <n v="19"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="1"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="6"/>
+    <n v="27"/>
+    <n v="3"/>
+    <n v="30"/>
+    <n v="24"/>
+    <s v="2018-10-14T17:00:00.000Z"/>
+  </r>
+  <r>
+    <x v="86"/>
+    <n v="2018"/>
+    <x v="5"/>
+    <x v="25"/>
+    <s v="Minnesota Vikings"/>
+    <n v="-10"/>
+    <n v="44"/>
+    <n v="14.91"/>
+    <n v="26.91"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="1"/>
+    <n v="0"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="17"/>
+    <n v="27"/>
+    <n v="44"/>
+    <n v="-10"/>
+    <s v="2018-10-14T17:00:00.000Z"/>
+  </r>
+  <r>
+    <x v="87"/>
+    <n v="2018"/>
+    <x v="5"/>
+    <x v="22"/>
+    <s v="New York Jets"/>
+    <n v="-2.5"/>
+    <n v="47.5"/>
+    <n v="20.27"/>
+    <n v="19.18"/>
+    <x v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="34"/>
+    <n v="42"/>
+    <n v="76"/>
+    <n v="-8"/>
+    <s v="2018-10-14T17:00:00.000Z"/>
+  </r>
+  <r>
+    <x v="88"/>
+    <n v="2018"/>
+    <x v="5"/>
+    <x v="15"/>
+    <s v="Denver Broncos"/>
+    <n v="6.5"/>
+    <n v="50.5"/>
+    <n v="30.91"/>
+    <n v="21.18"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
+    <n v="23"/>
+    <n v="20"/>
+    <n v="43"/>
+    <n v="3"/>
+    <s v="2018-10-14T20:05:00.000Z"/>
+  </r>
+  <r>
+    <x v="89"/>
+    <n v="2018"/>
+    <x v="5"/>
+    <x v="7"/>
+    <s v="Dallas Cowboys"/>
+    <n v="3"/>
+    <n v="40"/>
+    <n v="20.18"/>
+    <n v="20"/>
+    <x v="1"/>
+    <n v="0"/>
+    <n v="1"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="4"/>
+    <n v="7"/>
+    <n v="40"/>
+    <n v="47"/>
+    <n v="-33"/>
+    <s v="2018-10-14T20:25:00.000Z"/>
+  </r>
+  <r>
+    <x v="90"/>
+    <n v="2018"/>
+    <x v="5"/>
+    <x v="16"/>
+    <s v="Tennessee Titans"/>
+    <n v="2.5"/>
+    <n v="43"/>
+    <n v="23.27"/>
+    <n v="19"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="1"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="6"/>
+    <n v="21"/>
+    <n v="0"/>
+    <n v="21"/>
+    <n v="21"/>
+    <s v="2018-10-14T20:25:00.000Z"/>
+  </r>
+  <r>
+    <x v="91"/>
+    <n v="2018"/>
+    <x v="5"/>
+    <x v="9"/>
+    <s v="New England Patriots"/>
+    <n v="-3.5"/>
+    <n v="58.5"/>
+    <n v="30.73"/>
+    <n v="31.18"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="1"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="6"/>
+    <n v="40"/>
+    <n v="43"/>
+    <n v="83"/>
+    <n v="-3"/>
+    <s v="2018-10-15T00:20:00.000Z"/>
+  </r>
+  <r>
+    <x v="92"/>
+    <n v="2018"/>
+    <x v="5"/>
+    <x v="4"/>
+    <s v="Green Bay Packers"/>
+    <n v="-9"/>
+    <n v="46.5"/>
+    <n v="15.91"/>
+    <n v="29.55"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
+    <n v="30"/>
+    <n v="33"/>
+    <n v="63"/>
+    <n v="-3"/>
+    <s v="2018-10-16T00:15:00.000Z"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="18" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:E20" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="33" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:F19" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="21">
     <pivotField axis="axisRow" showAll="0">
-      <items count="49">
+      <items count="94">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
@@ -2133,16 +3279,101 @@
         <item x="45"/>
         <item x="46"/>
         <item x="47"/>
+        <item x="48"/>
+        <item x="49"/>
+        <item x="50"/>
+        <item x="51"/>
+        <item x="52"/>
+        <item x="53"/>
+        <item x="54"/>
+        <item x="55"/>
+        <item x="56"/>
+        <item x="57"/>
+        <item x="58"/>
+        <item x="59"/>
+        <item x="60"/>
+        <item x="61"/>
+        <item x="62"/>
+        <item x="63"/>
+        <item x="64"/>
+        <item x="65"/>
+        <item x="66"/>
+        <item x="67"/>
+        <item x="68"/>
+        <item x="69"/>
+        <item x="70"/>
+        <item x="71"/>
+        <item x="72"/>
+        <item x="73"/>
+        <item x="74"/>
+        <item x="75"/>
+        <item x="76"/>
+        <item x="77"/>
+        <item x="78"/>
+        <item x="79"/>
+        <item x="80"/>
+        <item x="81"/>
+        <item x="82"/>
+        <item x="83"/>
+        <item x="84"/>
+        <item x="85"/>
+        <item x="86"/>
+        <item x="87"/>
+        <item x="88"/>
+        <item x="89"/>
+        <item x="90"/>
+        <item x="91"/>
+        <item x="92"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField showAll="0"/>
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="4">
+      <items count="7">
         <item h="1" x="0"/>
         <item h="1" x="1"/>
-        <item x="2"/>
+        <item h="1" x="2"/>
+        <item h="1" x="3"/>
+        <item h="1" x="4"/>
+        <item x="5"/>
         <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="33">
+        <item sd="0" x="25"/>
+        <item sd="0" x="0"/>
+        <item sd="0" x="16"/>
+        <item sd="0" x="5"/>
+        <item sd="0" x="21"/>
+        <item sd="0" x="13"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="18"/>
+        <item sd="0" x="12"/>
+        <item sd="0" x="29"/>
+        <item sd="0" x="24"/>
+        <item sd="0" x="31"/>
+        <item sd="0" x="6"/>
+        <item sd="0" x="22"/>
+        <item sd="0" x="7"/>
+        <item sd="0" x="9"/>
+        <item sd="0" x="20"/>
+        <item sd="0" x="15"/>
+        <item sd="0" x="19"/>
+        <item sd="0" x="17"/>
+        <item sd="0" x="27"/>
+        <item sd="0" x="30"/>
+        <item sd="0" x="28"/>
+        <item sd="0" x="14"/>
+        <item sd="0" x="26"/>
+        <item sd="0" x="23"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="11"/>
+        <item sd="0" x="8"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="10"/>
+        <item t="default" sd="0"/>
       </items>
     </pivotField>
     <pivotField showAll="0"/>
@@ -2150,13 +3381,24 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
     <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -2164,57 +3406,55 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
   </pivotFields>
-  <rowFields count="1">
+  <rowFields count="2">
+    <field x="3"/>
     <field x="0"/>
   </rowFields>
-  <rowItems count="17">
+  <rowItems count="16">
     <i>
-      <x v="32"/>
+      <x/>
     </i>
     <i>
-      <x v="33"/>
+      <x v="2"/>
     </i>
     <i>
-      <x v="34"/>
+      <x v="3"/>
     </i>
     <i>
-      <x v="35"/>
+      <x v="4"/>
     </i>
     <i>
-      <x v="36"/>
+      <x v="5"/>
     </i>
     <i>
-      <x v="37"/>
+      <x v="13"/>
     </i>
     <i>
-      <x v="38"/>
+      <x v="14"/>
     </i>
     <i>
-      <x v="39"/>
+      <x v="15"/>
     </i>
     <i>
-      <x v="40"/>
+      <x v="16"/>
     </i>
     <i>
-      <x v="41"/>
+      <x v="17"/>
     </i>
     <i>
-      <x v="42"/>
+      <x v="25"/>
     </i>
     <i>
-      <x v="43"/>
+      <x v="26"/>
     </i>
     <i>
-      <x v="44"/>
+      <x v="27"/>
     </i>
     <i>
-      <x v="45"/>
+      <x v="28"/>
     </i>
     <i>
-      <x v="46"/>
-    </i>
-    <i>
-      <x v="47"/>
+      <x v="29"/>
     </i>
     <i t="grand">
       <x/>
@@ -2223,7 +3463,7 @@
   <colFields count="1">
     <field x="-2"/>
   </colFields>
-  <colItems count="4">
+  <colItems count="5">
     <i>
       <x/>
     </i>
@@ -2236,15 +3476,19 @@
     <i i="3">
       <x v="3"/>
     </i>
+    <i i="4">
+      <x v="4"/>
+    </i>
   </colItems>
   <pageFields count="1">
     <pageField fld="2" hier="-1"/>
   </pageFields>
-  <dataFields count="4">
+  <dataFields count="5">
     <dataField name="Sum of crowd.results.predictionScore" fld="15" baseField="0" baseItem="0"/>
+    <dataField name="Sum of crowd.results.spread.correct" fld="11" baseField="0" baseItem="0"/>
+    <dataField name="Sum of crowd.results.spread.push" fld="12" baseField="0" baseItem="0"/>
+    <dataField name="Sum of crowd.results.total.push" fld="14" baseField="0" baseItem="0"/>
     <dataField name="Sum of crowd.results.total.correct" fld="13" baseField="0" baseItem="0"/>
-    <dataField name="Sum of crowd.results.spread.correct" fld="11" baseField="0" baseItem="0"/>
-    <dataField name="Sum of crowd.results.winner.correct" fld="9" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -2259,8 +3503,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Games" displayName="Games" ref="A1:U78" totalsRowShown="0">
-  <autoFilter ref="A1:U78" xr:uid="{00000000-0009-0000-0100-000002000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Games" displayName="Games" ref="A1:U94" totalsRowShown="0">
+  <autoFilter ref="A1:U94" xr:uid="{00000000-0009-0000-0100-000002000000}">
     <filterColumn colId="2">
       <filters>
         <filter val="5"/>
@@ -2594,30 +3838,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:F98"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="27.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>72</v>
       </c>
@@ -2625,73 +3871,85 @@
         <v>74</v>
       </c>
       <c r="C3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F3" t="s">
         <v>75</v>
       </c>
-      <c r="D3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
-        <v>33</v>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="B4" s="3">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="3">
+        <v>6</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="3">
         <v>4</v>
       </c>
-      <c r="C4" s="3">
-        <v>1</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0</v>
-      </c>
-      <c r="E4" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
-        <v>34</v>
-      </c>
-      <c r="B5" s="3">
+      <c r="C6" s="3">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="3">
         <v>4</v>
       </c>
-      <c r="C5" s="3">
-        <v>0</v>
-      </c>
-      <c r="D5" s="3">
-        <v>1</v>
-      </c>
-      <c r="E5" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
-        <v>35</v>
-      </c>
-      <c r="B6" s="3">
-        <v>0</v>
-      </c>
-      <c r="C6" s="3">
-        <v>0</v>
-      </c>
-      <c r="D6" s="3">
-        <v>0</v>
-      </c>
-      <c r="E6" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
-        <v>36</v>
-      </c>
-      <c r="B7" s="3">
-        <v>2</v>
-      </c>
       <c r="C7" s="3">
         <v>1</v>
       </c>
@@ -2701,10 +3959,13 @@
       <c r="E7" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
-        <v>37</v>
+      <c r="F7" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="B8" s="3">
         <v>4</v>
@@ -2716,101 +3977,119 @@
         <v>0</v>
       </c>
       <c r="E8" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
-        <v>38</v>
+        <v>0</v>
+      </c>
+      <c r="F8" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="B9" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C9" s="3">
         <v>0</v>
       </c>
       <c r="D9" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
-        <v>39</v>
+      <c r="F9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="B10" s="3">
         <v>4</v>
       </c>
       <c r="C10" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="3">
+        <v>6</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="3">
+        <v>4</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="3">
+        <v>2</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="3">
-        <v>0</v>
-      </c>
-      <c r="C11" s="3">
-        <v>0</v>
-      </c>
-      <c r="D11" s="3">
-        <v>0</v>
-      </c>
-      <c r="E11" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
-        <v>41</v>
-      </c>
-      <c r="B12" s="3">
-        <v>2</v>
-      </c>
-      <c r="C12" s="3">
-        <v>0</v>
-      </c>
-      <c r="D12" s="3">
-        <v>0</v>
-      </c>
-      <c r="E12" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
-        <v>42</v>
-      </c>
-      <c r="B13" s="3">
+      <c r="B14" s="3">
         <v>4</v>
       </c>
-      <c r="C13" s="3">
-        <v>0</v>
-      </c>
-      <c r="D13" s="3">
-        <v>1</v>
-      </c>
-      <c r="E13" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
-        <v>43</v>
-      </c>
-      <c r="B14" s="3">
-        <v>2</v>
-      </c>
       <c r="C14" s="3">
         <v>1</v>
       </c>
@@ -2820,10 +4099,13 @@
       <c r="E14" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
-        <v>44</v>
+      <c r="F14" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="B15" s="3">
         <v>4</v>
@@ -2835,50 +4117,59 @@
         <v>0</v>
       </c>
       <c r="E15" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
-        <v>45</v>
+        <v>0</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="B16" s="3">
+        <v>2</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="3">
+        <v>6</v>
+      </c>
+      <c r="C17" s="3">
+        <v>1</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0</v>
+      </c>
+      <c r="F17" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="3">
         <v>4</v>
       </c>
-      <c r="C16" s="3">
-        <v>1</v>
-      </c>
-      <c r="D16" s="3">
-        <v>0</v>
-      </c>
-      <c r="E16" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
-        <v>46</v>
-      </c>
-      <c r="B17" s="3">
-        <v>4</v>
-      </c>
-      <c r="C17" s="3">
-        <v>0</v>
-      </c>
-      <c r="D17" s="3">
-        <v>1</v>
-      </c>
-      <c r="E17" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="2">
-        <v>47</v>
-      </c>
-      <c r="B18" s="3">
-        <v>2</v>
-      </c>
       <c r="C18" s="3">
         <v>1</v>
       </c>
@@ -2888,31 +4179,42 @@
       <c r="E18" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="2">
-        <v>48</v>
-      </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+      <c r="F18" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B20" s="3">
-        <v>42</v>
-      </c>
-      <c r="C20" s="3">
-        <v>7</v>
-      </c>
-      <c r="D20" s="3">
-        <v>5</v>
-      </c>
-      <c r="E20" s="3">
-        <v>9</v>
+      <c r="B19" s="3">
+        <v>56</v>
+      </c>
+      <c r="C19" s="3">
+        <v>11</v>
+      </c>
+      <c r="D19" s="3">
+        <v>1</v>
+      </c>
+      <c r="E19" s="3">
+        <v>1</v>
+      </c>
+      <c r="F19" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="98" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C98">
+        <f>46/89</f>
+        <v>0.5168539325842697</v>
+      </c>
+      <c r="E98">
+        <f>56/93</f>
+        <v>0.60215053763440862</v>
+      </c>
+      <c r="F98">
+        <f>47/92</f>
+        <v>0.51086956521739135</v>
       </c>
     </row>
   </sheetData>
@@ -2922,10 +4224,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:U78"/>
+  <dimension ref="A1:U94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I74" sqref="I74"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A79" sqref="A79:U94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6198,7 +7500,7 @@
         <v>-7</v>
       </c>
       <c r="U50" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="51" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
@@ -6263,7 +7565,7 @@
         <v>-2</v>
       </c>
       <c r="U51" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="52" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
@@ -6328,7 +7630,7 @@
         <v>-22</v>
       </c>
       <c r="U52" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="53" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
@@ -6393,7 +7695,7 @@
         <v>3</v>
       </c>
       <c r="U53" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="54" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
@@ -6458,7 +7760,7 @@
         <v>-38</v>
       </c>
       <c r="U54" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="55" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
@@ -6523,7 +7825,7 @@
         <v>1</v>
       </c>
       <c r="U55" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="56" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
@@ -6588,7 +7890,7 @@
         <v>-19</v>
       </c>
       <c r="U56" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="57" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
@@ -6653,7 +7955,7 @@
         <v>-3</v>
       </c>
       <c r="U57" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="58" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
@@ -6718,7 +8020,7 @@
         <v>-31</v>
       </c>
       <c r="U58" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="59" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
@@ -6783,7 +8085,7 @@
         <v>3</v>
       </c>
       <c r="U59" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="60" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
@@ -6848,7 +8150,7 @@
         <v>-3</v>
       </c>
       <c r="U60" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="61" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
@@ -6913,7 +8215,7 @@
         <v>15</v>
       </c>
       <c r="U61" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="62" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
@@ -6978,7 +8280,7 @@
         <v>-2</v>
       </c>
       <c r="U62" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="63" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
@@ -7043,7 +8345,7 @@
         <v>12</v>
       </c>
       <c r="U63" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="64" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
@@ -7108,7 +8410,7 @@
         <v>4</v>
       </c>
       <c r="U64" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="65" spans="1:21" x14ac:dyDescent="0.2">
@@ -7173,7 +8475,7 @@
         <v>-14</v>
       </c>
       <c r="U65" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="66" spans="1:21" x14ac:dyDescent="0.2">
@@ -7238,7 +8540,7 @@
         <v>-10</v>
       </c>
       <c r="U66" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="67" spans="1:21" x14ac:dyDescent="0.2">
@@ -7303,7 +8605,7 @@
         <v>-3</v>
       </c>
       <c r="U67" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="68" spans="1:21" x14ac:dyDescent="0.2">
@@ -7368,7 +8670,7 @@
         <v>-2</v>
       </c>
       <c r="U68" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="69" spans="1:21" x14ac:dyDescent="0.2">
@@ -7433,7 +8735,7 @@
         <v>-1</v>
       </c>
       <c r="U69" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="70" spans="1:21" x14ac:dyDescent="0.2">
@@ -7498,7 +8800,7 @@
         <v>-8</v>
       </c>
       <c r="U70" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="71" spans="1:21" x14ac:dyDescent="0.2">
@@ -7563,7 +8865,7 @@
         <v>-24</v>
       </c>
       <c r="U71" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="72" spans="1:21" x14ac:dyDescent="0.2">
@@ -7628,7 +8930,7 @@
         <v>-18</v>
       </c>
       <c r="U72" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="73" spans="1:21" x14ac:dyDescent="0.2">
@@ -7693,7 +8995,7 @@
         <v>-16</v>
       </c>
       <c r="U73" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="74" spans="1:21" x14ac:dyDescent="0.2">
@@ -7758,7 +9060,7 @@
         <v>-16</v>
       </c>
       <c r="U74" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="75" spans="1:21" x14ac:dyDescent="0.2">
@@ -7823,7 +9125,7 @@
         <v>10</v>
       </c>
       <c r="U75" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="76" spans="1:21" x14ac:dyDescent="0.2">
@@ -7888,7 +9190,7 @@
         <v>2</v>
       </c>
       <c r="U76" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="77" spans="1:21" x14ac:dyDescent="0.2">
@@ -7953,7 +9255,7 @@
         <v>2</v>
       </c>
       <c r="U77" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="78" spans="1:21" x14ac:dyDescent="0.2">
@@ -8018,7 +9320,1047 @@
         <v>-3</v>
       </c>
       <c r="U78" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="79" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79">
+        <v>2018</v>
+      </c>
+      <c r="C79">
+        <v>5</v>
+      </c>
+      <c r="D79" t="s">
+        <v>38</v>
+      </c>
+      <c r="E79" t="s">
+        <v>33</v>
+      </c>
+      <c r="F79">
+        <v>-6</v>
+      </c>
+      <c r="G79">
+        <v>52.5</v>
+      </c>
+      <c r="H79">
+        <v>22.53</v>
+      </c>
+      <c r="I79">
+        <v>30</v>
+      </c>
+      <c r="J79">
+        <v>1</v>
+      </c>
+      <c r="K79">
+        <v>0</v>
+      </c>
+      <c r="L79">
+        <v>1</v>
+      </c>
+      <c r="M79">
+        <v>0</v>
+      </c>
+      <c r="N79">
+        <v>1</v>
+      </c>
+      <c r="O79">
+        <v>0</v>
+      </c>
+      <c r="P79">
+        <v>6</v>
+      </c>
+      <c r="Q79">
+        <v>19</v>
+      </c>
+      <c r="R79">
+        <v>43</v>
+      </c>
+      <c r="S79">
+        <v>62</v>
+      </c>
+      <c r="T79">
+        <v>-24</v>
+      </c>
+      <c r="U79" t="s">
         <v>88</v>
+      </c>
+    </row>
+    <row r="80" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80">
+        <v>2018</v>
+      </c>
+      <c r="C80">
+        <v>6</v>
+      </c>
+      <c r="D80" t="s">
+        <v>40</v>
+      </c>
+      <c r="E80" t="s">
+        <v>27</v>
+      </c>
+      <c r="F80">
+        <v>1.5</v>
+      </c>
+      <c r="G80">
+        <v>44</v>
+      </c>
+      <c r="H80">
+        <v>23.75</v>
+      </c>
+      <c r="I80">
+        <v>19.63</v>
+      </c>
+      <c r="J80">
+        <v>1</v>
+      </c>
+      <c r="K80">
+        <v>0</v>
+      </c>
+      <c r="L80">
+        <v>1</v>
+      </c>
+      <c r="M80">
+        <v>0</v>
+      </c>
+      <c r="N80">
+        <v>0</v>
+      </c>
+      <c r="O80">
+        <v>0</v>
+      </c>
+      <c r="P80">
+        <v>4</v>
+      </c>
+      <c r="Q80">
+        <v>34</v>
+      </c>
+      <c r="R80">
+        <v>13</v>
+      </c>
+      <c r="S80">
+        <v>47</v>
+      </c>
+      <c r="T80">
+        <v>21</v>
+      </c>
+      <c r="U80" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="81" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81">
+        <v>2018</v>
+      </c>
+      <c r="C81">
+        <v>6</v>
+      </c>
+      <c r="D81" t="s">
+        <v>45</v>
+      </c>
+      <c r="E81" t="s">
+        <v>22</v>
+      </c>
+      <c r="F81">
+        <v>-1</v>
+      </c>
+      <c r="G81">
+        <v>47</v>
+      </c>
+      <c r="H81">
+        <v>23</v>
+      </c>
+      <c r="I81">
+        <v>20.73</v>
+      </c>
+      <c r="J81">
+        <v>1</v>
+      </c>
+      <c r="K81">
+        <v>0</v>
+      </c>
+      <c r="L81">
+        <v>1</v>
+      </c>
+      <c r="M81">
+        <v>0</v>
+      </c>
+      <c r="N81">
+        <v>0</v>
+      </c>
+      <c r="O81">
+        <v>0</v>
+      </c>
+      <c r="P81">
+        <v>4</v>
+      </c>
+      <c r="Q81">
+        <v>38</v>
+      </c>
+      <c r="R81">
+        <v>14</v>
+      </c>
+      <c r="S81">
+        <v>52</v>
+      </c>
+      <c r="T81">
+        <v>24</v>
+      </c>
+      <c r="U81" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="82" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82">
+        <v>2018</v>
+      </c>
+      <c r="C82">
+        <v>6</v>
+      </c>
+      <c r="D82" t="s">
+        <v>43</v>
+      </c>
+      <c r="E82" t="s">
+        <v>28</v>
+      </c>
+      <c r="F82">
+        <v>-10</v>
+      </c>
+      <c r="G82">
+        <v>40</v>
+      </c>
+      <c r="H82">
+        <v>16.45</v>
+      </c>
+      <c r="I82">
+        <v>23.64</v>
+      </c>
+      <c r="J82">
+        <v>1</v>
+      </c>
+      <c r="K82">
+        <v>0</v>
+      </c>
+      <c r="L82">
+        <v>1</v>
+      </c>
+      <c r="M82">
+        <v>0</v>
+      </c>
+      <c r="N82">
+        <v>0</v>
+      </c>
+      <c r="O82">
+        <v>0</v>
+      </c>
+      <c r="P82">
+        <v>4</v>
+      </c>
+      <c r="Q82">
+        <v>13</v>
+      </c>
+      <c r="R82">
+        <v>20</v>
+      </c>
+      <c r="S82">
+        <v>33</v>
+      </c>
+      <c r="T82">
+        <v>-7</v>
+      </c>
+      <c r="U82" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="83" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83">
+        <v>2018</v>
+      </c>
+      <c r="C83">
+        <v>6</v>
+      </c>
+      <c r="D83" t="s">
+        <v>56</v>
+      </c>
+      <c r="E83" t="s">
+        <v>24</v>
+      </c>
+      <c r="F83">
+        <v>-1.5</v>
+      </c>
+      <c r="G83">
+        <v>50</v>
+      </c>
+      <c r="H83">
+        <v>28.8</v>
+      </c>
+      <c r="I83">
+        <v>28</v>
+      </c>
+      <c r="J83">
+        <v>1</v>
+      </c>
+      <c r="K83">
+        <v>0</v>
+      </c>
+      <c r="L83">
+        <v>1</v>
+      </c>
+      <c r="M83">
+        <v>0</v>
+      </c>
+      <c r="N83">
+        <v>0</v>
+      </c>
+      <c r="O83">
+        <v>0</v>
+      </c>
+      <c r="P83">
+        <v>4</v>
+      </c>
+      <c r="Q83">
+        <v>28</v>
+      </c>
+      <c r="R83">
+        <v>21</v>
+      </c>
+      <c r="S83">
+        <v>49</v>
+      </c>
+      <c r="T83">
+        <v>7</v>
+      </c>
+      <c r="U83" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="84" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84">
+        <v>2018</v>
+      </c>
+      <c r="C84">
+        <v>6</v>
+      </c>
+      <c r="D84" t="s">
+        <v>57</v>
+      </c>
+      <c r="E84" t="s">
+        <v>34</v>
+      </c>
+      <c r="F84">
+        <v>-3</v>
+      </c>
+      <c r="G84">
+        <v>57.5</v>
+      </c>
+      <c r="H84">
+        <v>22.73</v>
+      </c>
+      <c r="I84">
+        <v>28.45</v>
+      </c>
+      <c r="J84">
+        <v>1</v>
+      </c>
+      <c r="K84">
+        <v>0</v>
+      </c>
+      <c r="L84">
+        <v>1</v>
+      </c>
+      <c r="M84">
+        <v>0</v>
+      </c>
+      <c r="N84">
+        <v>0</v>
+      </c>
+      <c r="O84">
+        <v>0</v>
+      </c>
+      <c r="P84">
+        <v>4</v>
+      </c>
+      <c r="Q84">
+        <v>29</v>
+      </c>
+      <c r="R84">
+        <v>34</v>
+      </c>
+      <c r="S84">
+        <v>63</v>
+      </c>
+      <c r="T84">
+        <v>-5</v>
+      </c>
+      <c r="U84" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="85" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85">
+        <v>2018</v>
+      </c>
+      <c r="C85">
+        <v>6</v>
+      </c>
+      <c r="D85" t="s">
+        <v>48</v>
+      </c>
+      <c r="E85" t="s">
+        <v>42</v>
+      </c>
+      <c r="F85">
+        <v>5.5</v>
+      </c>
+      <c r="G85">
+        <v>41.5</v>
+      </c>
+      <c r="H85">
+        <v>22.82</v>
+      </c>
+      <c r="I85">
+        <v>19.36</v>
+      </c>
+      <c r="J85">
+        <v>0</v>
+      </c>
+      <c r="K85">
+        <v>0</v>
+      </c>
+      <c r="L85">
+        <v>1</v>
+      </c>
+      <c r="M85">
+        <v>0</v>
+      </c>
+      <c r="N85">
+        <v>1</v>
+      </c>
+      <c r="O85">
+        <v>0</v>
+      </c>
+      <c r="P85">
+        <v>4</v>
+      </c>
+      <c r="Q85">
+        <v>28</v>
+      </c>
+      <c r="R85">
+        <v>31</v>
+      </c>
+      <c r="S85">
+        <v>59</v>
+      </c>
+      <c r="T85">
+        <v>-3</v>
+      </c>
+      <c r="U85" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="86" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86">
+        <v>2018</v>
+      </c>
+      <c r="C86">
+        <v>6</v>
+      </c>
+      <c r="D86" t="s">
+        <v>25</v>
+      </c>
+      <c r="E86" t="s">
+        <v>38</v>
+      </c>
+      <c r="F86">
+        <v>1</v>
+      </c>
+      <c r="G86">
+        <v>44.5</v>
+      </c>
+      <c r="H86">
+        <v>21.64</v>
+      </c>
+      <c r="I86">
+        <v>21</v>
+      </c>
+      <c r="J86">
+        <v>0</v>
+      </c>
+      <c r="K86">
+        <v>0</v>
+      </c>
+      <c r="L86">
+        <v>1</v>
+      </c>
+      <c r="M86">
+        <v>0</v>
+      </c>
+      <c r="N86">
+        <v>1</v>
+      </c>
+      <c r="O86">
+        <v>0</v>
+      </c>
+      <c r="P86">
+        <v>4</v>
+      </c>
+      <c r="Q86">
+        <v>17</v>
+      </c>
+      <c r="R86">
+        <v>23</v>
+      </c>
+      <c r="S86">
+        <v>40</v>
+      </c>
+      <c r="T86">
+        <v>-6</v>
+      </c>
+      <c r="U86" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="87" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87">
+        <v>2018</v>
+      </c>
+      <c r="C87">
+        <v>6</v>
+      </c>
+      <c r="D87" t="s">
+        <v>52</v>
+      </c>
+      <c r="E87" t="s">
+        <v>41</v>
+      </c>
+      <c r="F87">
+        <v>3</v>
+      </c>
+      <c r="G87">
+        <v>48</v>
+      </c>
+      <c r="H87">
+        <v>26.82</v>
+      </c>
+      <c r="I87">
+        <v>19</v>
+      </c>
+      <c r="J87">
+        <v>1</v>
+      </c>
+      <c r="K87">
+        <v>0</v>
+      </c>
+      <c r="L87">
+        <v>1</v>
+      </c>
+      <c r="M87">
+        <v>0</v>
+      </c>
+      <c r="N87">
+        <v>1</v>
+      </c>
+      <c r="O87">
+        <v>0</v>
+      </c>
+      <c r="P87">
+        <v>6</v>
+      </c>
+      <c r="Q87">
+        <v>27</v>
+      </c>
+      <c r="R87">
+        <v>3</v>
+      </c>
+      <c r="S87">
+        <v>30</v>
+      </c>
+      <c r="T87">
+        <v>24</v>
+      </c>
+      <c r="U87" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="88" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="B88">
+        <v>2018</v>
+      </c>
+      <c r="C88">
+        <v>6</v>
+      </c>
+      <c r="D88" t="s">
+        <v>49</v>
+      </c>
+      <c r="E88" t="s">
+        <v>44</v>
+      </c>
+      <c r="F88">
+        <v>-10</v>
+      </c>
+      <c r="G88">
+        <v>44</v>
+      </c>
+      <c r="H88">
+        <v>14.91</v>
+      </c>
+      <c r="I88">
+        <v>26.91</v>
+      </c>
+      <c r="J88">
+        <v>1</v>
+      </c>
+      <c r="K88">
+        <v>0</v>
+      </c>
+      <c r="L88">
+        <v>0</v>
+      </c>
+      <c r="M88">
+        <v>1</v>
+      </c>
+      <c r="N88">
+        <v>0</v>
+      </c>
+      <c r="O88">
+        <v>1</v>
+      </c>
+      <c r="P88">
+        <v>2</v>
+      </c>
+      <c r="Q88">
+        <v>17</v>
+      </c>
+      <c r="R88">
+        <v>27</v>
+      </c>
+      <c r="S88">
+        <v>44</v>
+      </c>
+      <c r="T88">
+        <v>-10</v>
+      </c>
+      <c r="U88" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="89" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89">
+        <v>2018</v>
+      </c>
+      <c r="C89">
+        <v>6</v>
+      </c>
+      <c r="D89" t="s">
+        <v>39</v>
+      </c>
+      <c r="E89" t="s">
+        <v>21</v>
+      </c>
+      <c r="F89">
+        <v>-2.5</v>
+      </c>
+      <c r="G89">
+        <v>47.5</v>
+      </c>
+      <c r="H89">
+        <v>20.27</v>
+      </c>
+      <c r="I89">
+        <v>19.18</v>
+      </c>
+      <c r="J89">
+        <v>0</v>
+      </c>
+      <c r="K89">
+        <v>0</v>
+      </c>
+      <c r="L89">
+        <v>0</v>
+      </c>
+      <c r="M89">
+        <v>0</v>
+      </c>
+      <c r="N89">
+        <v>0</v>
+      </c>
+      <c r="O89">
+        <v>0</v>
+      </c>
+      <c r="P89">
+        <v>0</v>
+      </c>
+      <c r="Q89">
+        <v>34</v>
+      </c>
+      <c r="R89">
+        <v>42</v>
+      </c>
+      <c r="S89">
+        <v>76</v>
+      </c>
+      <c r="T89">
+        <v>-8</v>
+      </c>
+      <c r="U89" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="90" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>89</v>
+      </c>
+      <c r="B90">
+        <v>2018</v>
+      </c>
+      <c r="C90">
+        <v>6</v>
+      </c>
+      <c r="D90" t="s">
+        <v>46</v>
+      </c>
+      <c r="E90" t="s">
+        <v>31</v>
+      </c>
+      <c r="F90">
+        <v>6.5</v>
+      </c>
+      <c r="G90">
+        <v>50.5</v>
+      </c>
+      <c r="H90">
+        <v>30.91</v>
+      </c>
+      <c r="I90">
+        <v>21.18</v>
+      </c>
+      <c r="J90">
+        <v>1</v>
+      </c>
+      <c r="K90">
+        <v>0</v>
+      </c>
+      <c r="L90">
+        <v>0</v>
+      </c>
+      <c r="M90">
+        <v>0</v>
+      </c>
+      <c r="N90">
+        <v>0</v>
+      </c>
+      <c r="O90">
+        <v>0</v>
+      </c>
+      <c r="P90">
+        <v>2</v>
+      </c>
+      <c r="Q90">
+        <v>23</v>
+      </c>
+      <c r="R90">
+        <v>20</v>
+      </c>
+      <c r="S90">
+        <v>43</v>
+      </c>
+      <c r="T90">
+        <v>3</v>
+      </c>
+      <c r="U90" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="91" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>90</v>
+      </c>
+      <c r="B91">
+        <v>2018</v>
+      </c>
+      <c r="C91">
+        <v>6</v>
+      </c>
+      <c r="D91" t="s">
+        <v>30</v>
+      </c>
+      <c r="E91" t="s">
+        <v>51</v>
+      </c>
+      <c r="F91">
+        <v>3</v>
+      </c>
+      <c r="G91">
+        <v>40</v>
+      </c>
+      <c r="H91">
+        <v>20.18</v>
+      </c>
+      <c r="I91">
+        <v>20</v>
+      </c>
+      <c r="J91">
+        <v>0</v>
+      </c>
+      <c r="K91">
+        <v>0</v>
+      </c>
+      <c r="L91">
+        <v>1</v>
+      </c>
+      <c r="M91">
+        <v>0</v>
+      </c>
+      <c r="N91">
+        <v>1</v>
+      </c>
+      <c r="O91">
+        <v>0</v>
+      </c>
+      <c r="P91">
+        <v>4</v>
+      </c>
+      <c r="Q91">
+        <v>7</v>
+      </c>
+      <c r="R91">
+        <v>40</v>
+      </c>
+      <c r="S91">
+        <v>47</v>
+      </c>
+      <c r="T91">
+        <v>-33</v>
+      </c>
+      <c r="U91" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="92" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="B92">
+        <v>2018</v>
+      </c>
+      <c r="C92">
+        <v>6</v>
+      </c>
+      <c r="D92" t="s">
+        <v>32</v>
+      </c>
+      <c r="E92" t="s">
+        <v>29</v>
+      </c>
+      <c r="F92">
+        <v>2.5</v>
+      </c>
+      <c r="G92">
+        <v>43</v>
+      </c>
+      <c r="H92">
+        <v>23.27</v>
+      </c>
+      <c r="I92">
+        <v>19</v>
+      </c>
+      <c r="J92">
+        <v>1</v>
+      </c>
+      <c r="K92">
+        <v>0</v>
+      </c>
+      <c r="L92">
+        <v>1</v>
+      </c>
+      <c r="M92">
+        <v>0</v>
+      </c>
+      <c r="N92">
+        <v>1</v>
+      </c>
+      <c r="O92">
+        <v>0</v>
+      </c>
+      <c r="P92">
+        <v>6</v>
+      </c>
+      <c r="Q92">
+        <v>21</v>
+      </c>
+      <c r="R92">
+        <v>0</v>
+      </c>
+      <c r="S92">
+        <v>21</v>
+      </c>
+      <c r="T92">
+        <v>21</v>
+      </c>
+      <c r="U92" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="93" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>92</v>
+      </c>
+      <c r="B93">
+        <v>2018</v>
+      </c>
+      <c r="C93">
+        <v>6</v>
+      </c>
+      <c r="D93" t="s">
+        <v>36</v>
+      </c>
+      <c r="E93" t="s">
+        <v>53</v>
+      </c>
+      <c r="F93">
+        <v>-3.5</v>
+      </c>
+      <c r="G93">
+        <v>58.5</v>
+      </c>
+      <c r="H93">
+        <v>30.73</v>
+      </c>
+      <c r="I93">
+        <v>31.18</v>
+      </c>
+      <c r="J93">
+        <v>1</v>
+      </c>
+      <c r="K93">
+        <v>0</v>
+      </c>
+      <c r="L93">
+        <v>1</v>
+      </c>
+      <c r="M93">
+        <v>0</v>
+      </c>
+      <c r="N93">
+        <v>1</v>
+      </c>
+      <c r="O93">
+        <v>0</v>
+      </c>
+      <c r="P93">
+        <v>6</v>
+      </c>
+      <c r="Q93">
+        <v>40</v>
+      </c>
+      <c r="R93">
+        <v>43</v>
+      </c>
+      <c r="S93">
+        <v>83</v>
+      </c>
+      <c r="T93">
+        <v>-3</v>
+      </c>
+      <c r="U93" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="94" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>93</v>
+      </c>
+      <c r="B94">
+        <v>2018</v>
+      </c>
+      <c r="C94">
+        <v>6</v>
+      </c>
+      <c r="D94" t="s">
+        <v>35</v>
+      </c>
+      <c r="E94" t="s">
+        <v>37</v>
+      </c>
+      <c r="F94">
+        <v>-9</v>
+      </c>
+      <c r="G94">
+        <v>46.5</v>
+      </c>
+      <c r="H94">
+        <v>15.91</v>
+      </c>
+      <c r="I94">
+        <v>29.55</v>
+      </c>
+      <c r="J94">
+        <v>1</v>
+      </c>
+      <c r="K94">
+        <v>0</v>
+      </c>
+      <c r="L94">
+        <v>0</v>
+      </c>
+      <c r="M94">
+        <v>0</v>
+      </c>
+      <c r="N94">
+        <v>0</v>
+      </c>
+      <c r="O94">
+        <v>0</v>
+      </c>
+      <c r="P94">
+        <v>2</v>
+      </c>
+      <c r="Q94">
+        <v>30</v>
+      </c>
+      <c r="R94">
+        <v>33</v>
+      </c>
+      <c r="S94">
+        <v>63</v>
+      </c>
+      <c r="T94">
+        <v>-3</v>
+      </c>
+      <c r="U94" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>